<commit_message>
fixed R1 and R4 values
</commit_message>
<xml_diff>
--- a/EDA/SMT/quack-bom.xlsx
+++ b/EDA/SMT/quack-bom.xlsx
@@ -157,22 +157,22 @@
     <t>C17561</t>
   </si>
   <si>
-    <t>150Ω ±1% 1/8W</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>C17471</t>
-  </si>
-  <si>
     <t>470Ω ±1% 1/8W</t>
   </si>
   <si>
-    <t>R2 R3 R4 R6 R7</t>
+    <t>R1 R2 R3 R6 R7</t>
   </si>
   <si>
     <t>C17710</t>
+  </si>
+  <si>
+    <t>1.2kΩ ±1% 1/8W</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>C17379</t>
   </si>
   <si>
     <t>100NF 50V</t>

</xml_diff>